<commit_message>
First commit with all working scripts. Need to add all bash script into a run_all_scripts.sh
</commit_message>
<xml_diff>
--- a/Sequencing_summary.xlsx
+++ b/Sequencing_summary.xlsx
@@ -21,9 +21,9 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filtre 2" guid="{ABAF8179-7069-4EDD-8B6D-7B212D31DE7A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filtre 1" guid="{E822526C-85B6-40C8-B392-D8D3E4EF0044}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="TALL only" guid="{8FC6A298-7499-43C0-B9C5-40410DA2B0F7}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filtre 1" guid="{E822526C-85B6-40C8-B392-D8D3E4EF0044}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filtre 2" guid="{ABAF8179-7069-4EDD-8B6D-7B212D31DE7A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2285" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="961">
   <si>
     <t>README</t>
   </si>
@@ -2877,49 +2877,85 @@
     <t>Run_252_NS500-159_29_03_2019_RC</t>
   </si>
   <si>
+    <t>S002829_1</t>
+  </si>
+  <si>
+    <t>S002828_1</t>
+  </si>
+  <si>
+    <t>/gpfs/tgml/reads/bcl/Run_252_190329_NS500637_0159_AHYGNKBGX9</t>
+  </si>
+  <si>
+    <t>/gpfs/tgml/reads/bcl/Run_309_200224_NS500637_0216_AH2J22BGXF</t>
+  </si>
+  <si>
+    <t>/gpfs/tgml/reads/bcl/Run_306_200214_NS500637_0213_AH23C3BGXF</t>
+  </si>
+  <si>
+    <t>mRNA_Hashtag_R306</t>
+  </si>
+  <si>
+    <t>mRNA_Hashtag_R309</t>
+  </si>
+  <si>
+    <t>HTO_Hashtag_R309</t>
+  </si>
+  <si>
+    <t>HTO_Hashtag_R306</t>
+  </si>
+  <si>
+    <t>CBF_R252</t>
+  </si>
+  <si>
+    <t>CBF_R255</t>
+  </si>
+  <si>
+    <t>FLT3_R252</t>
+  </si>
+  <si>
+    <t>Nicolas_Ginet</t>
+  </si>
+  <si>
+    <t>/gpfs/tgml/reads/bcl/Run_255_190408_NS500637_0162_AH7K2JBGXB</t>
+  </si>
+  <si>
+    <t>Total_seq_A</t>
+  </si>
+  <si>
+    <t>Total_seq_B</t>
+  </si>
+  <si>
+    <t>HTO1,GTCAACTCTTTAGCG;HTO2,TGATGGCCTATTGGG</t>
+  </si>
+  <si>
+    <t>Expected_cell_number</t>
+  </si>
+  <si>
+    <t>S003959</t>
+  </si>
+  <si>
+    <t>/gpfs/tgml/reads/NS500_output_from_sept_2020/Run_342_NS500-249_11-12-2020_LM</t>
+  </si>
+  <si>
+    <t>Run_342_NS500-249_11-12-2020_LM</t>
+  </si>
+  <si>
+    <t>SI-GA-A3</t>
+  </si>
+  <si>
+    <t>S003960</t>
+  </si>
+  <si>
+    <t>D701_S</t>
+  </si>
+  <si>
+    <t>mRNA_Hashtag_R342</t>
+  </si>
+  <si>
     <t>27x56</t>
   </si>
   <si>
-    <t>S002829_1</t>
-  </si>
-  <si>
-    <t>S002828_1</t>
-  </si>
-  <si>
-    <t>/gpfs/tgml/reads/bcl/Run_252_190329_NS500637_0159_AHYGNKBGX9</t>
-  </si>
-  <si>
-    <t>/gpfs/tgml/reads/bcl/Run_309_200224_NS500637_0216_AH2J22BGXF</t>
-  </si>
-  <si>
-    <t>/gpfs/tgml/reads/bcl/Run_306_200214_NS500637_0213_AH23C3BGXF</t>
-  </si>
-  <si>
-    <t>mRNA_Hashtag_R306</t>
-  </si>
-  <si>
-    <t>mRNA_Hashtag_R309</t>
-  </si>
-  <si>
-    <t>HTO_Hashtag_R309</t>
-  </si>
-  <si>
-    <t>HTO_Hashtag_R306</t>
-  </si>
-  <si>
-    <t>CBF_R252</t>
-  </si>
-  <si>
-    <t>CBF_R255</t>
-  </si>
-  <si>
-    <t>FLT3_R252</t>
-  </si>
-  <si>
-    <t>Nicolas_Ginet</t>
-  </si>
-  <si>
-    <t>/gpfs/tgml/reads/bcl/Run_255_190408_NS500637_0162_AH7K2JBGXB</t>
+    <t>HTO_Hashtag_R342</t>
   </si>
 </sst>
 </file>
@@ -2930,7 +2966,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3082,6 +3118,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3113,7 +3154,7 @@
     <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3253,6 +3294,8 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="4" builtinId="8"/>
@@ -3261,7 +3304,7 @@
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="252">
+  <dxfs count="253">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4404,234 +4447,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF3F3F3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0E0E3"/>
-          <bgColor rgb="FFD0E0E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF3F3F3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0E0E3"/>
-          <bgColor rgb="FFD0E0E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -5460,6 +5275,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -5804,6 +5637,234 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF3F3F3"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF3F3F3"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
@@ -5828,9 +5889,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="samples-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="251"/>
-      <tableStyleElement type="firstRowStripe" dxfId="250"/>
-      <tableStyleElement type="secondRowStripe" dxfId="249"/>
+      <tableStyleElement type="headerRow" dxfId="252"/>
+      <tableStyleElement type="firstRowStripe" dxfId="251"/>
+      <tableStyleElement type="secondRowStripe" dxfId="250"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -5842,96 +5903,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:CG11" headerRowCount="0" headerRowDxfId="248" dataDxfId="247" totalsRowDxfId="246">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:CH13" headerRowCount="0" headerRowDxfId="222" dataDxfId="221" totalsRowDxfId="220">
   <sortState ref="A1:CG1540">
     <sortCondition ref="I2"/>
   </sortState>
-  <tableColumns count="85">
-    <tableColumn id="1" name="Column1" dataDxfId="245"/>
-    <tableColumn id="2" name="Column2" dataDxfId="244"/>
-    <tableColumn id="3" name="Column3" dataDxfId="243"/>
-    <tableColumn id="4" name="Column4" dataDxfId="242"/>
-    <tableColumn id="5" name="Column5" dataDxfId="241"/>
-    <tableColumn id="6" name="Column6" dataDxfId="240"/>
-    <tableColumn id="7" name="Column7" dataDxfId="239"/>
-    <tableColumn id="8" name="Column8" dataDxfId="238"/>
-    <tableColumn id="9" name="Column9" dataDxfId="237"/>
-    <tableColumn id="82" name="Colonne1" dataDxfId="236"/>
-    <tableColumn id="10" name="Column10" dataDxfId="235"/>
-    <tableColumn id="11" name="Column11" dataDxfId="234"/>
-    <tableColumn id="12" name="Column12" dataDxfId="233"/>
-    <tableColumn id="13" name="Column13" dataDxfId="232"/>
-    <tableColumn id="14" name="Column14" dataDxfId="231"/>
-    <tableColumn id="15" name="Column15" dataDxfId="230"/>
-    <tableColumn id="16" name="Column16" dataDxfId="229"/>
-    <tableColumn id="17" name="Column17" dataDxfId="228"/>
-    <tableColumn id="18" name="Column18" dataDxfId="227"/>
-    <tableColumn id="19" name="Column19" dataDxfId="226"/>
-    <tableColumn id="20" name="Column20" dataDxfId="225"/>
-    <tableColumn id="21" name="Column21" dataDxfId="224"/>
-    <tableColumn id="22" name="Column22" dataDxfId="223"/>
-    <tableColumn id="85" name="Colonne5" dataDxfId="222"/>
-    <tableColumn id="84" name="Colonne4" dataDxfId="221"/>
-    <tableColumn id="81" name="Colonne3" dataDxfId="220"/>
-    <tableColumn id="83" name="Colonne2" dataDxfId="219"/>
-    <tableColumn id="23" name="Column23" dataDxfId="218"/>
-    <tableColumn id="24" name="Column24" dataDxfId="217"/>
-    <tableColumn id="25" name="Column25" dataDxfId="216"/>
-    <tableColumn id="26" name="Column26" dataDxfId="215"/>
-    <tableColumn id="27" name="Column27" dataDxfId="214"/>
-    <tableColumn id="28" name="Column28" dataDxfId="213"/>
-    <tableColumn id="29" name="Column29" dataDxfId="212"/>
-    <tableColumn id="30" name="Column30" dataDxfId="211"/>
-    <tableColumn id="31" name="Column31" dataDxfId="210"/>
-    <tableColumn id="32" name="Column32" dataDxfId="209"/>
-    <tableColumn id="33" name="Column33" dataDxfId="208"/>
-    <tableColumn id="34" name="Column34" dataDxfId="207"/>
-    <tableColumn id="35" name="Column35" dataDxfId="206"/>
-    <tableColumn id="36" name="Column36" dataDxfId="205"/>
-    <tableColumn id="37" name="Column37" dataDxfId="204"/>
-    <tableColumn id="38" name="Column38" dataDxfId="203"/>
-    <tableColumn id="39" name="Column39" dataDxfId="202"/>
-    <tableColumn id="40" name="Column40" dataDxfId="201"/>
-    <tableColumn id="41" name="Column41" dataDxfId="200"/>
-    <tableColumn id="42" name="Column42" dataDxfId="199"/>
-    <tableColumn id="43" name="Column43" dataDxfId="198"/>
-    <tableColumn id="44" name="Column44" dataDxfId="197"/>
-    <tableColumn id="45" name="Column45" dataDxfId="196"/>
-    <tableColumn id="46" name="Column46" dataDxfId="195"/>
-    <tableColumn id="47" name="Column47" dataDxfId="194"/>
-    <tableColumn id="48" name="Column48" dataDxfId="193"/>
-    <tableColumn id="49" name="Column49" dataDxfId="192"/>
-    <tableColumn id="50" name="Column50" dataDxfId="191"/>
-    <tableColumn id="51" name="Column51" dataDxfId="190"/>
-    <tableColumn id="52" name="Column52" dataDxfId="189"/>
-    <tableColumn id="53" name="Column53" dataDxfId="188"/>
-    <tableColumn id="54" name="Column54" dataDxfId="187"/>
-    <tableColumn id="55" name="Column55" dataDxfId="186"/>
-    <tableColumn id="56" name="Column56" dataDxfId="185"/>
-    <tableColumn id="57" name="Column57" dataDxfId="184"/>
-    <tableColumn id="58" name="Column58" dataDxfId="183"/>
-    <tableColumn id="59" name="Column59" dataDxfId="182"/>
-    <tableColumn id="60" name="Column60" dataDxfId="181"/>
-    <tableColumn id="61" name="Column61" dataDxfId="180"/>
-    <tableColumn id="62" name="Column62" dataDxfId="179"/>
-    <tableColumn id="63" name="Column63" dataDxfId="178"/>
-    <tableColumn id="64" name="Column64" dataDxfId="177"/>
-    <tableColumn id="65" name="Column65" dataDxfId="176"/>
-    <tableColumn id="66" name="Column66" dataDxfId="175"/>
-    <tableColumn id="67" name="Column67" dataDxfId="174"/>
-    <tableColumn id="68" name="Column68" dataDxfId="173"/>
-    <tableColumn id="69" name="Column69" dataDxfId="172"/>
-    <tableColumn id="70" name="Column70" dataDxfId="171"/>
-    <tableColumn id="71" name="Column71" dataDxfId="170"/>
-    <tableColumn id="72" name="Column72" dataDxfId="169"/>
-    <tableColumn id="73" name="Column73" dataDxfId="168"/>
-    <tableColumn id="74" name="Column74" dataDxfId="167"/>
-    <tableColumn id="75" name="Column75" dataDxfId="166"/>
-    <tableColumn id="76" name="Column76" dataDxfId="165"/>
-    <tableColumn id="77" name="Column77" dataDxfId="164"/>
-    <tableColumn id="78" name="Column78" dataDxfId="163"/>
-    <tableColumn id="79" name="Column79" dataDxfId="162"/>
-    <tableColumn id="80" name="Column80" dataDxfId="161"/>
+  <tableColumns count="86">
+    <tableColumn id="1" name="Column1" dataDxfId="219"/>
+    <tableColumn id="2" name="Column2" dataDxfId="218"/>
+    <tableColumn id="3" name="Column3" dataDxfId="217"/>
+    <tableColumn id="4" name="Column4" dataDxfId="216"/>
+    <tableColumn id="5" name="Column5" dataDxfId="215"/>
+    <tableColumn id="6" name="Column6" dataDxfId="214"/>
+    <tableColumn id="7" name="Column7" dataDxfId="213"/>
+    <tableColumn id="8" name="Column8" dataDxfId="212"/>
+    <tableColumn id="9" name="Column9" dataDxfId="211"/>
+    <tableColumn id="82" name="Colonne1" dataDxfId="210"/>
+    <tableColumn id="10" name="Column10" dataDxfId="209"/>
+    <tableColumn id="11" name="Column11" dataDxfId="208"/>
+    <tableColumn id="12" name="Column12" dataDxfId="207"/>
+    <tableColumn id="13" name="Column13" dataDxfId="206"/>
+    <tableColumn id="14" name="Column14" dataDxfId="205"/>
+    <tableColumn id="15" name="Column15" dataDxfId="204"/>
+    <tableColumn id="16" name="Column16" dataDxfId="203"/>
+    <tableColumn id="17" name="Column17" dataDxfId="202"/>
+    <tableColumn id="18" name="Column18" dataDxfId="201"/>
+    <tableColumn id="19" name="Column19" dataDxfId="200"/>
+    <tableColumn id="20" name="Column20" dataDxfId="199"/>
+    <tableColumn id="21" name="Column21" dataDxfId="198"/>
+    <tableColumn id="22" name="Column22" dataDxfId="197"/>
+    <tableColumn id="86" name="Colonne6" dataDxfId="196"/>
+    <tableColumn id="85" name="Colonne5" dataDxfId="195"/>
+    <tableColumn id="84" name="Colonne4" dataDxfId="194"/>
+    <tableColumn id="81" name="Colonne3" dataDxfId="193"/>
+    <tableColumn id="83" name="Colonne2" dataDxfId="192"/>
+    <tableColumn id="23" name="Column23" dataDxfId="191"/>
+    <tableColumn id="24" name="Column24" dataDxfId="190"/>
+    <tableColumn id="25" name="Column25" dataDxfId="189"/>
+    <tableColumn id="26" name="Column26" dataDxfId="188"/>
+    <tableColumn id="27" name="Column27" dataDxfId="187"/>
+    <tableColumn id="28" name="Column28" dataDxfId="186"/>
+    <tableColumn id="29" name="Column29" dataDxfId="185"/>
+    <tableColumn id="30" name="Column30" dataDxfId="184"/>
+    <tableColumn id="31" name="Column31" dataDxfId="183"/>
+    <tableColumn id="32" name="Column32" dataDxfId="182"/>
+    <tableColumn id="33" name="Column33" dataDxfId="181"/>
+    <tableColumn id="34" name="Column34" dataDxfId="180"/>
+    <tableColumn id="35" name="Column35" dataDxfId="179"/>
+    <tableColumn id="36" name="Column36" dataDxfId="178"/>
+    <tableColumn id="37" name="Column37" dataDxfId="177"/>
+    <tableColumn id="38" name="Column38" dataDxfId="176"/>
+    <tableColumn id="39" name="Column39" dataDxfId="175"/>
+    <tableColumn id="40" name="Column40" dataDxfId="174"/>
+    <tableColumn id="41" name="Column41" dataDxfId="173"/>
+    <tableColumn id="42" name="Column42" dataDxfId="172"/>
+    <tableColumn id="43" name="Column43" dataDxfId="171"/>
+    <tableColumn id="44" name="Column44" dataDxfId="170"/>
+    <tableColumn id="45" name="Column45" dataDxfId="169"/>
+    <tableColumn id="46" name="Column46" dataDxfId="168"/>
+    <tableColumn id="47" name="Column47" dataDxfId="167"/>
+    <tableColumn id="48" name="Column48" dataDxfId="166"/>
+    <tableColumn id="49" name="Column49" dataDxfId="165"/>
+    <tableColumn id="50" name="Column50" dataDxfId="164"/>
+    <tableColumn id="51" name="Column51" dataDxfId="163"/>
+    <tableColumn id="52" name="Column52" dataDxfId="162"/>
+    <tableColumn id="53" name="Column53" dataDxfId="161"/>
+    <tableColumn id="54" name="Column54" dataDxfId="160"/>
+    <tableColumn id="55" name="Column55" dataDxfId="159"/>
+    <tableColumn id="56" name="Column56" dataDxfId="158"/>
+    <tableColumn id="57" name="Column57" dataDxfId="157"/>
+    <tableColumn id="58" name="Column58" dataDxfId="156"/>
+    <tableColumn id="59" name="Column59" dataDxfId="155"/>
+    <tableColumn id="60" name="Column60" dataDxfId="154"/>
+    <tableColumn id="61" name="Column61" dataDxfId="153"/>
+    <tableColumn id="62" name="Column62" dataDxfId="152"/>
+    <tableColumn id="63" name="Column63" dataDxfId="151"/>
+    <tableColumn id="64" name="Column64" dataDxfId="150"/>
+    <tableColumn id="65" name="Column65" dataDxfId="149"/>
+    <tableColumn id="66" name="Column66" dataDxfId="148"/>
+    <tableColumn id="67" name="Column67" dataDxfId="147"/>
+    <tableColumn id="68" name="Column68" dataDxfId="146"/>
+    <tableColumn id="69" name="Column69" dataDxfId="145"/>
+    <tableColumn id="70" name="Column70" dataDxfId="144"/>
+    <tableColumn id="71" name="Column71" dataDxfId="143"/>
+    <tableColumn id="72" name="Column72" dataDxfId="142"/>
+    <tableColumn id="73" name="Column73" dataDxfId="141"/>
+    <tableColumn id="74" name="Column74" dataDxfId="140"/>
+    <tableColumn id="75" name="Column75" dataDxfId="139"/>
+    <tableColumn id="76" name="Column76" dataDxfId="138"/>
+    <tableColumn id="77" name="Column77" dataDxfId="137"/>
+    <tableColumn id="78" name="Column78" dataDxfId="136"/>
+    <tableColumn id="79" name="Column79" dataDxfId="135"/>
+    <tableColumn id="80" name="Column80" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="samples-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -29021,13 +29083,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CG11"/>
+  <dimension ref="A1:CH13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29054,49 +29116,49 @@
     <col min="20" max="20" width="9.140625" customWidth="1"/>
     <col min="21" max="21" width="4" customWidth="1"/>
     <col min="22" max="22" width="35.7109375" customWidth="1"/>
-    <col min="23" max="26" width="46.5703125" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" style="25" customWidth="1"/>
-    <col min="29" max="29" width="12.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9" style="25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11" style="25" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9" style="25" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.7109375" style="63" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.85546875" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" customWidth="1"/>
-    <col min="42" max="42" width="14.28515625" customWidth="1"/>
-    <col min="43" max="43" width="10.42578125" customWidth="1"/>
-    <col min="44" max="44" width="18.28515625" customWidth="1"/>
-    <col min="45" max="45" width="10.42578125" customWidth="1"/>
-    <col min="46" max="46" width="10.7109375" customWidth="1"/>
-    <col min="47" max="47" width="25.85546875" customWidth="1"/>
-    <col min="48" max="48" width="9.7109375" customWidth="1"/>
-    <col min="49" max="49" width="28.85546875" customWidth="1"/>
-    <col min="50" max="50" width="11.85546875" customWidth="1"/>
-    <col min="51" max="52" width="9.140625" customWidth="1"/>
-    <col min="53" max="53" width="8.7109375" customWidth="1"/>
-    <col min="54" max="54" width="9.140625" customWidth="1"/>
-    <col min="55" max="55" width="9.7109375" customWidth="1"/>
-    <col min="56" max="56" width="11.85546875" customWidth="1"/>
-    <col min="57" max="57" width="10.85546875" customWidth="1"/>
-    <col min="58" max="58" width="9.140625" customWidth="1"/>
-    <col min="59" max="59" width="11.140625" customWidth="1"/>
-    <col min="60" max="60" width="9.28515625" customWidth="1"/>
-    <col min="61" max="61" width="10.140625" customWidth="1"/>
-    <col min="62" max="62" width="9.85546875" customWidth="1"/>
-    <col min="63" max="63" width="13" customWidth="1"/>
-    <col min="64" max="64" width="11.7109375" customWidth="1"/>
-    <col min="65" max="65" width="10.42578125" customWidth="1"/>
-    <col min="66" max="85" width="8.140625" customWidth="1"/>
+    <col min="23" max="27" width="46.5703125" customWidth="1"/>
+    <col min="28" max="28" width="24.7109375" customWidth="1"/>
+    <col min="29" max="29" width="15.7109375" style="25" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9" style="25" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" style="25" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9" style="25" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" style="63" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.85546875" customWidth="1"/>
+    <col min="42" max="42" width="10.42578125" customWidth="1"/>
+    <col min="43" max="43" width="14.28515625" customWidth="1"/>
+    <col min="44" max="44" width="10.42578125" customWidth="1"/>
+    <col min="45" max="45" width="18.28515625" customWidth="1"/>
+    <col min="46" max="46" width="10.42578125" customWidth="1"/>
+    <col min="47" max="47" width="10.7109375" customWidth="1"/>
+    <col min="48" max="48" width="25.85546875" customWidth="1"/>
+    <col min="49" max="49" width="9.7109375" customWidth="1"/>
+    <col min="50" max="50" width="28.85546875" customWidth="1"/>
+    <col min="51" max="51" width="11.85546875" customWidth="1"/>
+    <col min="52" max="53" width="9.140625" customWidth="1"/>
+    <col min="54" max="54" width="8.7109375" customWidth="1"/>
+    <col min="55" max="55" width="9.140625" customWidth="1"/>
+    <col min="56" max="56" width="9.7109375" customWidth="1"/>
+    <col min="57" max="57" width="11.85546875" customWidth="1"/>
+    <col min="58" max="58" width="10.85546875" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" customWidth="1"/>
+    <col min="60" max="60" width="11.140625" customWidth="1"/>
+    <col min="61" max="61" width="9.28515625" customWidth="1"/>
+    <col min="62" max="62" width="10.140625" customWidth="1"/>
+    <col min="63" max="63" width="9.85546875" customWidth="1"/>
+    <col min="64" max="64" width="13" customWidth="1"/>
+    <col min="65" max="65" width="11.7109375" customWidth="1"/>
+    <col min="66" max="66" width="10.42578125" customWidth="1"/>
+    <col min="67" max="86" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>3</v>
       </c>
@@ -29167,57 +29229,59 @@
         <v>24</v>
       </c>
       <c r="X1" s="45" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y1" s="45" t="s">
         <v>914</v>
       </c>
-      <c r="Y1" s="45" t="s">
+      <c r="Z1" s="45" t="s">
         <v>915</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="AA1" s="45" t="s">
         <v>916</v>
       </c>
-      <c r="AA1" s="45" t="s">
+      <c r="AB1" s="45" t="s">
         <v>841</v>
       </c>
-      <c r="AB1" s="43" t="s">
+      <c r="AC1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="43" t="s">
+      <c r="AD1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="43" t="s">
+      <c r="AE1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="43" t="s">
+      <c r="AF1" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="43" t="s">
+      <c r="AG1" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="43" t="s">
+      <c r="AH1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="46" t="s">
+      <c r="AI1" s="46" t="s">
         <v>783</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="60" t="s">
+      <c r="AK1" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="45" t="s">
+      <c r="AL1" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="45" t="s">
+      <c r="AM1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="45" t="s">
+      <c r="AN1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="45"/>
       <c r="AO1" s="45"/>
       <c r="AP1" s="45"/>
-      <c r="AQ1" s="41"/>
+      <c r="AQ1" s="45"/>
       <c r="AR1" s="41"/>
       <c r="AS1" s="41"/>
       <c r="AT1" s="41"/>
@@ -29260,21 +29324,22 @@
       <c r="CE1" s="41"/>
       <c r="CF1" s="41"/>
       <c r="CG1" s="41"/>
-    </row>
-    <row r="2" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH1" s="41"/>
+    </row>
+    <row r="2" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45">
         <v>1</v>
       </c>
       <c r="B2" s="41" t="str">
-        <f>CONCATENATE(E2, "_", D2)</f>
+        <f t="shared" ref="B2:B8" si="0">CONCATENATE(E2, "_", D2)</f>
         <v>S002828_1_FLT3_R252</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="44" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
@@ -29297,7 +29362,7 @@
         <v>111</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="O2" s="41"/>
       <c r="P2" s="47">
@@ -29316,40 +29381,40 @@
       <c r="W2" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="45"/>
+      <c r="X2" s="54"/>
       <c r="Y2" s="45"/>
       <c r="Z2" s="45"/>
-      <c r="AA2" s="45" t="s">
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="AB2" s="44" t="s">
+      <c r="AC2" s="44" t="s">
         <v>931</v>
       </c>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="55">
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="55">
         <v>8</v>
       </c>
-      <c r="AE2" s="44"/>
       <c r="AF2" s="44"/>
       <c r="AG2" s="44"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="45">
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="48"/>
+      <c r="AJ2" s="45">
         <v>1</v>
       </c>
-      <c r="AJ2" s="61">
+      <c r="AK2" s="61">
         <v>1</v>
       </c>
-      <c r="AK2" s="57" t="s">
+      <c r="AL2" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="AL2" s="50"/>
-      <c r="AM2" s="45" t="s">
-        <v>934</v>
-      </c>
-      <c r="AN2" s="45"/>
+      <c r="AM2" s="50"/>
+      <c r="AN2" s="45" t="s">
+        <v>959</v>
+      </c>
       <c r="AO2" s="45"/>
       <c r="AP2" s="45"/>
-      <c r="AQ2" s="41"/>
+      <c r="AQ2" s="45"/>
       <c r="AR2" s="41"/>
       <c r="AS2" s="41"/>
       <c r="AT2" s="41"/>
@@ -29392,21 +29457,22 @@
       <c r="CE2" s="41"/>
       <c r="CF2" s="41"/>
       <c r="CG2" s="41"/>
-    </row>
-    <row r="3" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH2" s="41"/>
+    </row>
+    <row r="3" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45">
         <v>2</v>
       </c>
       <c r="B3" s="41" t="str">
-        <f>CONCATENATE(E3, "_", D3)</f>
+        <f t="shared" si="0"/>
         <v>S002829_1_CBF_R252</v>
       </c>
       <c r="C3" s="41"/>
       <c r="D3" s="44" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
@@ -29429,7 +29495,7 @@
         <v>111</v>
       </c>
       <c r="N3" s="44" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="47">
@@ -29448,40 +29514,40 @@
       <c r="W3" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="45"/>
+      <c r="X3" s="54"/>
       <c r="Y3" s="45"/>
       <c r="Z3" s="45"/>
-      <c r="AA3" s="45" t="s">
+      <c r="AA3" s="45"/>
+      <c r="AB3" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="AB3" s="44" t="s">
+      <c r="AC3" s="44" t="s">
         <v>932</v>
       </c>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="55">
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="55">
         <v>8</v>
       </c>
-      <c r="AE3" s="44"/>
       <c r="AF3" s="44"/>
       <c r="AG3" s="44"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="45">
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="45">
         <v>1</v>
       </c>
-      <c r="AJ3" s="61">
+      <c r="AK3" s="61">
         <v>2</v>
       </c>
-      <c r="AK3" s="57" t="s">
+      <c r="AL3" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="AL3" s="50"/>
-      <c r="AM3" s="45" t="s">
-        <v>934</v>
-      </c>
-      <c r="AN3" s="45"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="45" t="s">
+        <v>959</v>
+      </c>
       <c r="AO3" s="45"/>
       <c r="AP3" s="45"/>
-      <c r="AQ3" s="41"/>
+      <c r="AQ3" s="45"/>
       <c r="AR3" s="41"/>
       <c r="AS3" s="41"/>
       <c r="AT3" s="41"/>
@@ -29524,18 +29590,19 @@
       <c r="CE3" s="41"/>
       <c r="CF3" s="41"/>
       <c r="CG3" s="41"/>
-    </row>
-    <row r="4" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH3" s="41"/>
+    </row>
+    <row r="4" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45">
         <v>3</v>
       </c>
       <c r="B4" s="41" t="str">
-        <f>CONCATENATE(E4, "_", D4)</f>
+        <f t="shared" si="0"/>
         <v>S002829_CBF_R255</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="44" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="E4" s="44" t="s">
         <v>75</v>
@@ -29561,7 +29628,7 @@
         <v>111</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="47">
@@ -29583,37 +29650,37 @@
       <c r="X4" s="45"/>
       <c r="Y4" s="45"/>
       <c r="Z4" s="45"/>
-      <c r="AA4" s="45" t="s">
+      <c r="AA4" s="45"/>
+      <c r="AB4" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="AB4" s="44" t="s">
+      <c r="AC4" s="44" t="s">
         <v>932</v>
       </c>
-      <c r="AC4" s="44"/>
-      <c r="AD4" s="55">
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="55">
         <v>8</v>
       </c>
-      <c r="AE4" s="44"/>
       <c r="AF4" s="44"/>
       <c r="AG4" s="44"/>
-      <c r="AH4" s="48"/>
-      <c r="AI4" s="45">
+      <c r="AH4" s="44"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="45">
         <v>1</v>
       </c>
-      <c r="AJ4" s="61">
+      <c r="AK4" s="61">
         <v>1</v>
       </c>
-      <c r="AK4" s="57" t="s">
+      <c r="AL4" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="AL4" s="50"/>
-      <c r="AM4" s="45" t="s">
+      <c r="AM4" s="50"/>
+      <c r="AN4" s="45" t="s">
         <v>777</v>
       </c>
-      <c r="AN4" s="45"/>
       <c r="AO4" s="45"/>
       <c r="AP4" s="45"/>
-      <c r="AQ4" s="41"/>
+      <c r="AQ4" s="45"/>
       <c r="AR4" s="41"/>
       <c r="AS4" s="41"/>
       <c r="AT4" s="41"/>
@@ -29656,18 +29723,19 @@
       <c r="CE4" s="41"/>
       <c r="CF4" s="41"/>
       <c r="CG4" s="41"/>
-    </row>
-    <row r="5" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH4" s="41"/>
+    </row>
+    <row r="5" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="45">
         <v>4</v>
       </c>
       <c r="B5" s="41" t="str">
-        <f>CONCATENATE(E5, "_", D5)</f>
+        <f t="shared" si="0"/>
         <v>S003718_19_3_HTO_Hashtag_R306</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="52" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="E5" s="52" t="s">
         <v>780</v>
@@ -29693,7 +29761,7 @@
         <v>111</v>
       </c>
       <c r="N5" s="52" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="O5" s="51"/>
       <c r="P5" s="53">
@@ -29712,40 +29780,46 @@
       <c r="W5" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="X5" s="54"/>
+      <c r="X5" s="54">
+        <v>10000</v>
+      </c>
       <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="55" t="s">
+      <c r="Z5" s="54" t="s">
+        <v>950</v>
+      </c>
+      <c r="AA5" s="54" t="s">
+        <v>948</v>
+      </c>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="AC5" s="55" t="s">
+      <c r="AD5" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="AD5" s="55">
+      <c r="AE5" s="55">
         <v>8</v>
       </c>
-      <c r="AE5" s="56"/>
       <c r="AF5" s="56"/>
       <c r="AG5" s="56"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="45">
+      <c r="AH5" s="56"/>
+      <c r="AI5" s="48"/>
+      <c r="AJ5" s="45">
         <v>1</v>
       </c>
-      <c r="AJ5" s="62">
+      <c r="AK5" s="62">
         <v>1</v>
       </c>
-      <c r="AK5" s="57" t="s">
+      <c r="AL5" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="54" t="s">
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="54" t="s">
         <v>777</v>
       </c>
-      <c r="AN5" s="54"/>
       <c r="AO5" s="54"/>
       <c r="AP5" s="54"/>
-      <c r="AQ5" s="51"/>
+      <c r="AQ5" s="54"/>
       <c r="AR5" s="51"/>
       <c r="AS5" s="51"/>
       <c r="AT5" s="51"/>
@@ -29788,18 +29862,19 @@
       <c r="CE5" s="51"/>
       <c r="CF5" s="51"/>
       <c r="CG5" s="51"/>
-    </row>
-    <row r="6" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH5" s="51"/>
+    </row>
+    <row r="6" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45">
         <v>5</v>
       </c>
       <c r="B6" s="41" t="str">
-        <f>CONCATENATE(E6, "_", D6)</f>
+        <f t="shared" si="0"/>
         <v>S003718_19_4_mRNA_Hashtag_R306</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="52" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>781</v>
@@ -29825,7 +29900,7 @@
         <v>111</v>
       </c>
       <c r="N6" s="52" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="O6" s="51"/>
       <c r="P6" s="53">
@@ -29847,37 +29922,37 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="54"/>
       <c r="Z6" s="54"/>
-      <c r="AA6" s="54" t="s">
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="AB6" s="55" t="s">
+      <c r="AC6" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="AC6" s="55"/>
-      <c r="AD6" s="55">
+      <c r="AD6" s="55"/>
+      <c r="AE6" s="55">
         <v>8</v>
       </c>
-      <c r="AE6" s="56"/>
       <c r="AF6" s="56"/>
       <c r="AG6" s="56"/>
-      <c r="AH6" s="48"/>
-      <c r="AI6" s="45">
+      <c r="AH6" s="56"/>
+      <c r="AI6" s="48"/>
+      <c r="AJ6" s="45">
         <v>1</v>
       </c>
-      <c r="AJ6" s="62">
+      <c r="AK6" s="62">
         <v>2</v>
       </c>
-      <c r="AK6" s="57" t="s">
+      <c r="AL6" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="AL6" s="58"/>
-      <c r="AM6" s="54" t="s">
+      <c r="AM6" s="58"/>
+      <c r="AN6" s="54" t="s">
         <v>777</v>
       </c>
-      <c r="AN6" s="54"/>
       <c r="AO6" s="54"/>
       <c r="AP6" s="54"/>
-      <c r="AQ6" s="51"/>
+      <c r="AQ6" s="54"/>
       <c r="AR6" s="51"/>
       <c r="AS6" s="51"/>
       <c r="AT6" s="51"/>
@@ -29920,18 +29995,19 @@
       <c r="CE6" s="51"/>
       <c r="CF6" s="51"/>
       <c r="CG6" s="51"/>
-    </row>
-    <row r="7" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH6" s="51"/>
+    </row>
+    <row r="7" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45">
         <v>6</v>
       </c>
       <c r="B7" s="41" t="str">
-        <f>CONCATENATE(E7, "_", D7)</f>
+        <f t="shared" si="0"/>
         <v>S003718_19_1_HTO_Hashtag_R309</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="44" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E7" s="44" t="s">
         <v>778</v>
@@ -29957,7 +30033,7 @@
         <v>111</v>
       </c>
       <c r="N7" s="44" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="47">
@@ -29976,40 +30052,46 @@
       <c r="W7" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="X7" s="45"/>
+      <c r="X7" s="45">
+        <v>10000</v>
+      </c>
       <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="44" t="s">
+      <c r="Z7" s="54" t="s">
+        <v>950</v>
+      </c>
+      <c r="AA7" s="54" t="s">
+        <v>948</v>
+      </c>
+      <c r="AB7" s="45"/>
+      <c r="AC7" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="AC7" s="44" t="s">
+      <c r="AD7" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="AD7" s="44">
+      <c r="AE7" s="44">
         <v>8</v>
       </c>
-      <c r="AE7" s="44"/>
       <c r="AF7" s="44"/>
       <c r="AG7" s="44"/>
-      <c r="AH7" s="48"/>
-      <c r="AI7" s="45">
+      <c r="AH7" s="44"/>
+      <c r="AI7" s="48"/>
+      <c r="AJ7" s="45">
         <v>1</v>
       </c>
-      <c r="AJ7" s="61">
+      <c r="AK7" s="61">
         <v>1</v>
       </c>
-      <c r="AK7" s="49" t="s">
+      <c r="AL7" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="AL7" s="50"/>
-      <c r="AM7" s="45" t="s">
+      <c r="AM7" s="50"/>
+      <c r="AN7" s="45" t="s">
         <v>777</v>
       </c>
-      <c r="AN7" s="45"/>
       <c r="AO7" s="45"/>
       <c r="AP7" s="45"/>
-      <c r="AQ7" s="41"/>
+      <c r="AQ7" s="45"/>
       <c r="AR7" s="41"/>
       <c r="AS7" s="41"/>
       <c r="AT7" s="41"/>
@@ -30052,18 +30134,19 @@
       <c r="CE7" s="41"/>
       <c r="CF7" s="41"/>
       <c r="CG7" s="41"/>
-    </row>
-    <row r="8" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH7" s="41"/>
+    </row>
+    <row r="8" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45">
         <v>7</v>
       </c>
       <c r="B8" s="41" t="str">
-        <f>CONCATENATE(E8, "_", D8)</f>
+        <f t="shared" si="0"/>
         <v>S003718_19_2_mRNA_Hashtag_R309</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="44" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E8" s="44" t="s">
         <v>779</v>
@@ -30089,7 +30172,7 @@
         <v>111</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="O8" s="41"/>
       <c r="P8" s="47">
@@ -30111,37 +30194,37 @@
       <c r="X8" s="41"/>
       <c r="Y8" s="41"/>
       <c r="Z8" s="41"/>
-      <c r="AA8" s="41" t="s">
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="AB8" s="44" t="s">
+      <c r="AC8" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="AC8" s="44"/>
-      <c r="AD8" s="44">
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="44">
         <v>8</v>
       </c>
-      <c r="AE8" s="44"/>
       <c r="AF8" s="44"/>
       <c r="AG8" s="44"/>
-      <c r="AH8" s="48"/>
-      <c r="AI8" s="45">
+      <c r="AH8" s="44"/>
+      <c r="AI8" s="48"/>
+      <c r="AJ8" s="45">
         <v>1</v>
       </c>
-      <c r="AJ8" s="61">
+      <c r="AK8" s="61">
         <v>2</v>
       </c>
-      <c r="AK8" s="49" t="s">
+      <c r="AL8" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="AL8" s="50"/>
-      <c r="AM8" s="45" t="s">
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="45" t="s">
         <v>777</v>
       </c>
-      <c r="AN8" s="45"/>
       <c r="AO8" s="45"/>
       <c r="AP8" s="45"/>
-      <c r="AQ8" s="41"/>
+      <c r="AQ8" s="45"/>
       <c r="AR8" s="41"/>
       <c r="AS8" s="41"/>
       <c r="AT8" s="41"/>
@@ -30184,13 +30267,14 @@
       <c r="CE8" s="41"/>
       <c r="CF8" s="41"/>
       <c r="CG8" s="41"/>
-    </row>
-    <row r="9" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH8" s="41"/>
+    </row>
+    <row r="9" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="45">
         <v>8</v>
       </c>
       <c r="B9" s="41" t="str">
-        <f t="shared" ref="B9:B11" si="0">CONCATENATE(E9, "_", D9)</f>
+        <f t="shared" ref="B9:B13" si="1">CONCATENATE(E9, "_", D9)</f>
         <v>S004186_P8_ARNm</v>
       </c>
       <c r="C9" s="25"/>
@@ -30241,31 +30325,31 @@
       <c r="X9" s="59"/>
       <c r="Y9" s="59"/>
       <c r="Z9" s="59"/>
-      <c r="AA9" s="43" t="s">
+      <c r="AA9" s="59"/>
+      <c r="AB9" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="AB9" s="25" t="s">
+      <c r="AC9" s="25" t="s">
         <v>880</v>
       </c>
-      <c r="AD9" s="25">
+      <c r="AE9" s="25">
         <v>8</v>
       </c>
-      <c r="AI9" s="25">
+      <c r="AJ9" s="25">
         <v>1</v>
       </c>
-      <c r="AJ9" s="64">
+      <c r="AK9" s="64">
         <v>1</v>
       </c>
-      <c r="AK9" s="25" t="s">
+      <c r="AL9" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="AL9" s="65">
+      <c r="AM9" s="65">
         <v>44333</v>
       </c>
-      <c r="AM9" s="25" t="s">
+      <c r="AN9" s="25" t="s">
         <v>777</v>
       </c>
-      <c r="AN9" s="25"/>
       <c r="AO9" s="25"/>
       <c r="AP9" s="25"/>
       <c r="AQ9" s="25"/>
@@ -30311,13 +30395,14 @@
       <c r="CE9" s="25"/>
       <c r="CF9" s="25"/>
       <c r="CG9" s="25"/>
-    </row>
-    <row r="10" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH9" s="25"/>
+    </row>
+    <row r="10" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45">
         <v>9</v>
       </c>
       <c r="B10" s="41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>S004187_P13_ARNm</v>
       </c>
       <c r="C10" s="25"/>
@@ -30369,31 +30454,31 @@
       <c r="X10" s="59"/>
       <c r="Y10" s="59"/>
       <c r="Z10" s="59"/>
-      <c r="AA10" s="43" t="s">
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="AB10" s="25" t="s">
+      <c r="AC10" s="25" t="s">
         <v>881</v>
       </c>
-      <c r="AD10" s="25">
+      <c r="AE10" s="25">
         <v>8</v>
       </c>
-      <c r="AI10" s="25">
+      <c r="AJ10" s="25">
         <v>1</v>
       </c>
-      <c r="AJ10" s="64">
+      <c r="AK10" s="64">
         <v>2</v>
       </c>
-      <c r="AK10" s="25" t="s">
+      <c r="AL10" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="AL10" s="65">
+      <c r="AM10" s="65">
         <v>44333</v>
       </c>
-      <c r="AM10" s="25" t="s">
+      <c r="AN10" s="25" t="s">
         <v>777</v>
       </c>
-      <c r="AN10" s="25"/>
       <c r="AO10" s="25"/>
       <c r="AP10" s="25"/>
       <c r="AQ10" s="25"/>
@@ -30439,13 +30524,14 @@
       <c r="CE10" s="25"/>
       <c r="CF10" s="25"/>
       <c r="CG10" s="25"/>
-    </row>
-    <row r="11" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH10" s="25"/>
+    </row>
+    <row r="11" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45">
         <v>10</v>
       </c>
       <c r="B11" s="41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>S004266_3_P8bis_ARNm</v>
       </c>
       <c r="C11" s="25"/>
@@ -30496,28 +30582,33 @@
       <c r="X11" s="67"/>
       <c r="Y11" s="67"/>
       <c r="Z11" s="67"/>
-      <c r="AA11" s="43" t="s">
+      <c r="AA11" s="67"/>
+      <c r="AB11" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="AB11" s="25" t="s">
+      <c r="AC11" s="25" t="s">
         <v>872</v>
       </c>
-      <c r="AI11" s="25">
+      <c r="AE11" s="25">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="56"/>
+      <c r="AG11" s="56"/>
+      <c r="AJ11" s="25">
         <v>1</v>
       </c>
-      <c r="AJ11" s="64">
+      <c r="AK11" s="64">
         <v>1</v>
       </c>
-      <c r="AK11" s="25" t="s">
+      <c r="AL11" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="AL11" s="65">
+      <c r="AM11" s="65">
         <v>44383</v>
       </c>
-      <c r="AM11" s="25" t="s">
+      <c r="AN11" s="25" t="s">
         <v>777</v>
       </c>
-      <c r="AN11" s="25"/>
       <c r="AO11" s="25"/>
       <c r="AP11" s="25"/>
       <c r="AQ11" s="25"/>
@@ -30563,12 +30654,187 @@
       <c r="CE11" s="25"/>
       <c r="CF11" s="25"/>
       <c r="CG11" s="25"/>
+      <c r="CH11" s="25"/>
+    </row>
+    <row r="12" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="45">
+        <v>11</v>
+      </c>
+      <c r="B12" s="41" t="str">
+        <f t="shared" si="1"/>
+        <v>S003959_mRNA_Hashtag_R342</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>958</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>952</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>855</v>
+      </c>
+      <c r="K12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="N12" s="25" t="s">
+        <v>953</v>
+      </c>
+      <c r="P12">
+        <v>342</v>
+      </c>
+      <c r="S12" t="s">
+        <v>852</v>
+      </c>
+      <c r="V12" t="s">
+        <v>954</v>
+      </c>
+      <c r="W12" t="s">
+        <v>46</v>
+      </c>
+      <c r="X12" s="70"/>
+      <c r="Y12" s="70"/>
+      <c r="Z12" s="70"/>
+      <c r="AA12" s="70"/>
+      <c r="AB12" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC12" s="25" t="s">
+        <v>955</v>
+      </c>
+      <c r="AE12" s="25">
+        <v>8</v>
+      </c>
+      <c r="AF12" s="56"/>
+      <c r="AG12" s="56"/>
+      <c r="AJ12">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="63">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM12" s="69">
+        <v>44176</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="45">
+        <v>12</v>
+      </c>
+      <c r="B13" s="41" t="str">
+        <f t="shared" si="1"/>
+        <v>S003960_HTO_Hashtag_R342</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>960</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>956</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>855</v>
+      </c>
+      <c r="K13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="N13" s="25" t="s">
+        <v>953</v>
+      </c>
+      <c r="P13">
+        <v>342</v>
+      </c>
+      <c r="S13" t="s">
+        <v>852</v>
+      </c>
+      <c r="V13" t="s">
+        <v>954</v>
+      </c>
+      <c r="W13" t="s">
+        <v>46</v>
+      </c>
+      <c r="X13" s="70">
+        <v>10000</v>
+      </c>
+      <c r="Y13" s="70"/>
+      <c r="Z13" s="70" t="s">
+        <v>950</v>
+      </c>
+      <c r="AA13" s="54" t="s">
+        <v>948</v>
+      </c>
+      <c r="AB13" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC13" s="25" t="s">
+        <v>957</v>
+      </c>
+      <c r="AD13" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE13" s="25">
+        <v>8</v>
+      </c>
+      <c r="AF13" s="56"/>
+      <c r="AG13" s="56"/>
+      <c r="AJ13">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="63">
+        <v>2</v>
+      </c>
+      <c r="AL13" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM13" s="69">
+        <v>44176</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>777</v>
+      </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{8FC6A298-7499-43C0-B9C5-40410DA2B0F7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{ABAF8179-7069-4EDD-8B6D-7B212D31DE7A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="S1:S2"/>
+      <autoFilter ref="A1:AF1111">
+        <filterColumn colId="14">
+          <filters>
+            <filter val="310"/>
+            <filter val="313"/>
+            <filter val="314"/>
+            <filter val="315"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
     </customSheetView>
     <customSheetView guid="{E822526C-85B6-40C8-B392-D8D3E4EF0044}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30601,153 +30867,144 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{ABAF8179-7069-4EDD-8B6D-7B212D31DE7A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8FC6A298-7499-43C0-B9C5-40410DA2B0F7}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AF1111">
-        <filterColumn colId="14">
-          <filters>
-            <filter val="310"/>
-            <filter val="313"/>
-            <filter val="314"/>
-            <filter val="315"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="S1:S2"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="I1:I3 I5:I11">
-    <cfRule type="cellIs" dxfId="160" priority="629" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="629" operator="equal">
       <formula>"Unknown"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K3 K5:K11">
-    <cfRule type="cellIs" dxfId="159" priority="630" operator="equal">
+  <conditionalFormatting sqref="K1:K3 K5:K13">
+    <cfRule type="cellIs" dxfId="248" priority="630" operator="equal">
       <formula>"human"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K3 K5:K11">
-    <cfRule type="cellIs" dxfId="158" priority="631" operator="equal">
+  <conditionalFormatting sqref="K1:K3 K5:K13">
+    <cfRule type="cellIs" dxfId="247" priority="631" operator="equal">
       <formula>"mouse"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3 I5:I11">
-    <cfRule type="cellIs" dxfId="157" priority="632" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="632" operator="equal">
       <formula>"ChIP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L11">
-    <cfRule type="cellIs" dxfId="156" priority="633" operator="equal">
+  <conditionalFormatting sqref="L2:L13">
+    <cfRule type="cellIs" dxfId="245" priority="633" operator="equal">
       <formula>"pe"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L11">
-    <cfRule type="cellIs" dxfId="155" priority="634" operator="equal">
+  <conditionalFormatting sqref="L2:L13">
+    <cfRule type="cellIs" dxfId="244" priority="634" operator="equal">
       <formula>"se"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H11">
-    <cfRule type="cellIs" dxfId="154" priority="637" operator="equal">
+  <conditionalFormatting sqref="H1:H13">
+    <cfRule type="cellIs" dxfId="243" priority="637" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H11">
-    <cfRule type="cellIs" dxfId="153" priority="638" operator="equal">
+  <conditionalFormatting sqref="H1:H13">
+    <cfRule type="cellIs" dxfId="242" priority="638" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H11">
-    <cfRule type="cellIs" dxfId="152" priority="639" operator="equal">
+  <conditionalFormatting sqref="H1:H13">
+    <cfRule type="cellIs" dxfId="241" priority="639" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3 I5:I11">
-    <cfRule type="cellIs" dxfId="151" priority="640" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="640" operator="equal">
       <formula>"ATAC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3 I5:I11">
-    <cfRule type="cellIs" dxfId="150" priority="641" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="641" operator="equal">
       <formula>"DNASE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3 I5:I11">
-    <cfRule type="cellIs" dxfId="149" priority="642" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="642" operator="equal">
       <formula>"RNA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3 I5:I11">
-    <cfRule type="cellIs" dxfId="148" priority="643" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="643" operator="equal">
       <formula>"CapStarr"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K3 K5:K11">
-    <cfRule type="cellIs" dxfId="147" priority="644" operator="equal">
+  <conditionalFormatting sqref="K1:K3 K5:K13">
+    <cfRule type="cellIs" dxfId="236" priority="644" operator="equal">
       <formula>"xenopus"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11 G1:G2 G8:G9 G5">
-    <cfRule type="notContainsBlanks" dxfId="146" priority="646">
+    <cfRule type="notContainsBlanks" dxfId="235" priority="646">
       <formula>LEN(TRIM(G1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3 I5:I11">
-    <cfRule type="cellIs" dxfId="145" priority="648" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="648" operator="equal">
       <formula>"miRNA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="144" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="1" operator="equal">
       <formula>"Unknown"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="143" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="2" operator="equal">
       <formula>"human"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="142" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="3" operator="equal">
       <formula>"mouse"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="141" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="4" operator="equal">
       <formula>"ChIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="140" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="8" operator="equal">
       <formula>"ATAC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="139" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="9" operator="equal">
       <formula>"DNASE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="138" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="10" operator="equal">
       <formula>"RNA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="137" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="11" operator="equal">
       <formula>"CapStarr"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="136" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="12" operator="equal">
       <formula>"xenopus"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="notContainsBlanks" dxfId="135" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="224" priority="13">
       <formula>LEN(TRIM(G4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="134" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="14" operator="equal">
       <formula>"miRNA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30775,7 +31032,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A11">
+  <conditionalFormatting sqref="A1:A13">
     <cfRule type="colorScale" priority="889">
       <colorScale>
         <cfvo type="min"/>
@@ -30799,7 +31056,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>data_validation_lists!$F$2:$F$4</xm:f>
@@ -30834,13 +31091,19 @@
           <x14:formula1>
             <xm:f>data_validation_lists!$L$2:$L$28</xm:f>
           </x14:formula1>
-          <xm:sqref>W1:Z1048576</xm:sqref>
+          <xm:sqref>W1:W1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>data_validation_lists!$I$2:$I$50</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>data_validation_lists!$O$2:$O$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AA2:AA1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -30853,7 +31116,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30919,6 +31182,9 @@
       <c r="N1" s="24" t="s">
         <v>816</v>
       </c>
+      <c r="O1" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -30963,7 +31229,9 @@
       <c r="N2" s="7" t="s">
         <v>856</v>
       </c>
-      <c r="O2" s="7"/>
+      <c r="O2" s="7" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -31008,7 +31276,9 @@
       <c r="N3" s="7" t="s">
         <v>854</v>
       </c>
-      <c r="O3" s="7"/>
+      <c r="O3" s="7" t="s">
+        <v>949</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -31627,7 +31897,7 @@
         <v>43</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="K43" s="6"/>
     </row>

</xml_diff>